<commit_message>
Implemented link gene for recipient in NEC and some changess in MISC
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099MISCTemplate.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099MISCTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NaeemIqbal\Downloads\Excel sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\EvoTaxPortal\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD26971-58B3-4915-BC0B-7C758DAAED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593EACBF-6DE6-4B91-81F0-D12EB18A0BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="1099-MISC" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1099-MISC'!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -194,7 +197,7 @@
     <t>Box 18 Amount</t>
   </si>
   <si>
-    <t>Is Corrected</t>
+    <t>Is Corrected Form of 1099</t>
   </si>
 </sst>
 </file>
@@ -804,7 +807,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -849,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1176,7 +1182,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN2" sqref="AN2"/>
+      <selection pane="bottomLeft" activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,9 +1220,10 @@
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="12" customWidth="1"/>
     <col min="39" max="39" width="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1334,17 +1341,21 @@
       <c r="AM1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="23" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 AN1:AN1048576 N1:O1048576" xr:uid="{A7AFD029-1AB9-4C87-A215-8DFCBA5FFED1}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 N1:O1048576" xr:uid="{A7AFD029-1AB9-4C87-A215-8DFCBA5FFED1}">
       <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN1:AN1048576" xr:uid="{421FFDE5-BD47-465D-8E32-5C4C630CA100}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>